<commit_message>
Price maker/taker and nuclear case
</commit_message>
<xml_diff>
--- a/input_files/case_files/BTES_nuclear_CONUS.xlsx
+++ b/input_files/case_files/BTES_nuclear_CONUS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awongel/Projects/clab_borehole_th_storage/input_files/case_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/m_/v6c97p3x1mg6bmvchddj43dc0000gn/T/fz3temp-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5894258-D02C-A841-812B-3C8B771D971E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F13743-9B55-EC41-8FAA-8AF9739E51C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="116">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -353,9 +353,6 @@
     <t>heat_turbine</t>
   </si>
   <si>
-    <t>heat_to_heat</t>
-  </si>
-  <si>
     <t>#Link</t>
   </si>
   <si>
@@ -374,19 +371,16 @@
     <t>StorageUnit</t>
   </si>
   <si>
-    <t>heat_in</t>
-  </si>
-  <si>
-    <t>heat_out</t>
-  </si>
-  <si>
     <t>normalization</t>
   </si>
   <si>
     <t>db</t>
   </si>
   <si>
-    <t>natrium_charger</t>
+    <t>heat</t>
+  </si>
+  <si>
+    <t>#Store</t>
   </si>
 </sst>
 </file>
@@ -1294,10 +1288,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W73"/>
+  <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1307,7 +1301,7 @@
     <col min="4" max="4" width="10.1640625" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.1640625" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
     <col min="10" max="10" width="18.1640625" customWidth="1"/>
@@ -1315,9 +1309,9 @@
     <col min="12" max="12" width="11.1640625" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="15" max="16" width="11.5" customWidth="1"/>
-    <col min="17" max="17" width="14.1640625" customWidth="1"/>
-    <col min="18" max="18" width="11.1640625" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="17" max="18" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1576,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1584,7 +1578,7 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1759,7 +1753,7 @@
         <v>71</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>97</v>
@@ -1784,6 +1778,9 @@
       </c>
       <c r="Q49" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="R49" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
@@ -1803,7 +1800,7 @@
         <v>1</v>
       </c>
       <c r="H50" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J50" s="5"/>
       <c r="L50" s="5"/>
@@ -1876,7 +1873,7 @@
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B53" t="s">
         <v>21</v>
@@ -1902,7 +1899,7 @@
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B54" t="s">
         <v>77</v>
@@ -1928,7 +1925,7 @@
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B55" t="s">
         <v>80</v>
@@ -1954,7 +1951,7 @@
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B56" t="s">
         <v>85</v>
@@ -1988,7 +1985,7 @@
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B57" t="s">
         <v>89</v>
@@ -2021,12 +2018,15 @@
         <v>0.9</v>
       </c>
       <c r="P57" s="5"/>
+      <c r="R57">
+        <v>4</v>
+      </c>
       <c r="S57" s="5"/>
       <c r="W57" s="5"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
         <v>94</v>
@@ -2035,35 +2035,35 @@
         <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="E58" t="s">
         <v>83</v>
       </c>
       <c r="J58" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K58" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="L58" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M58" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="O58" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="B59" t="s">
         <v>82</v>
@@ -2072,17 +2072,17 @@
         <v>81</v>
       </c>
       <c r="D59" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="J59" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K59" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="L59" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M59" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
@@ -2092,15 +2092,15 @@
         <v>1</v>
       </c>
       <c r="O59" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="P59" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B60" t="s">
         <v>95</v>
@@ -2112,27 +2112,27 @@
         <v>83</v>
       </c>
       <c r="E60" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="J60" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K60" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
       <c r="L60" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="M60" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
       <c r="O60" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="P60" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
@@ -2164,7 +2164,7 @@
         <v>104</v>
       </c>
       <c r="D62" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J62" s="15">
         <f>0.020828805*1000*B34</f>
@@ -2176,117 +2176,81 @@
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D63" t="s">
-        <v>113</v>
-      </c>
-      <c r="E63" t="s">
-        <v>103</v>
-      </c>
-      <c r="J63" s="15"/>
-      <c r="L63" s="5"/>
+        <v>114</v>
+      </c>
+      <c r="J63" s="19">
+        <f>0.000254017*1000*B34</f>
+        <v>2225.1889200000001</v>
+      </c>
+      <c r="L63" s="17">
+        <f>0.00000000371*1000</f>
+        <v>3.7099999999999996E-6</v>
+      </c>
       <c r="O63" s="5"/>
       <c r="P63" s="5"/>
+      <c r="Q63" s="16">
+        <v>2.6153100000000001E-4</v>
+      </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D64" t="s">
-        <v>103</v>
+        <v>114</v>
+      </c>
+      <c r="E64" t="s">
+        <v>87</v>
       </c>
       <c r="J64" s="19">
-        <f>0.000254017*1000*B34</f>
-        <v>2225.1889200000001</v>
-      </c>
-      <c r="L64" s="17">
-        <f>0.00000000371*1000</f>
-        <v>3.7099999999999996E-6</v>
-      </c>
-      <c r="O64" s="5"/>
-      <c r="P64" s="5"/>
-      <c r="Q64" s="16">
-        <v>2.6153100000000001E-4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65" t="s">
-        <v>106</v>
-      </c>
-      <c r="D65" t="s">
-        <v>103</v>
-      </c>
-      <c r="E65" t="s">
-        <v>114</v>
-      </c>
-      <c r="J65" s="15"/>
-      <c r="L65" s="5"/>
-      <c r="O65" s="5"/>
-      <c r="P65" s="5"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A66" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B66" t="s">
-        <v>105</v>
-      </c>
-      <c r="D66" t="s">
-        <v>114</v>
-      </c>
-      <c r="E66" t="s">
-        <v>87</v>
-      </c>
-      <c r="J66" s="19">
         <f>0.020905199*1000*B34</f>
         <v>183129.54324</v>
       </c>
-      <c r="L66" s="5"/>
-      <c r="O66" s="16">
+      <c r="L64" s="5"/>
+      <c r="O64" s="16">
         <v>0.37080028399999998</v>
       </c>
-      <c r="P66" s="5"/>
-    </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P64" s="5"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A70" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A72" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
         <v>59</v>
       </c>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update nuclear input file
</commit_message>
<xml_diff>
--- a/input_files/case_files/BTES_nuclear_CONUS.xlsx
+++ b/input_files/case_files/BTES_nuclear_CONUS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/folders/m_/v6c97p3x1mg6bmvchddj43dc0000gn/T/fz3temp-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F13743-9B55-EC41-8FAA-8AF9739E51C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFFE9A1-1F67-9546-81A5-FEA416EA2736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input_intermodel_one_node_" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="121">
   <si>
     <t>Note that demand has no decisions.</t>
   </si>
@@ -281,9 +281,6 @@
     <t>BTES</t>
   </si>
   <si>
-    <t>granite</t>
-  </si>
-  <si>
     <t>btes</t>
   </si>
   <si>
@@ -338,21 +335,9 @@
     <t>2019-01-01 00:00:00</t>
   </si>
   <si>
-    <t>20230922_US_mthd3_2010-2020_wind.csv</t>
-  </si>
-  <si>
-    <t>20230922_US_mthd3_2010-2020_solar.csv</t>
-  </si>
-  <si>
     <t>natrium</t>
   </si>
   <si>
-    <t>nuclear_heat</t>
-  </si>
-  <si>
-    <t>heat_turbine</t>
-  </si>
-  <si>
     <t>#Link</t>
   </si>
   <si>
@@ -365,9 +350,6 @@
     <t>btes_nuclear_output</t>
   </si>
   <si>
-    <t>US_demand_unnormalized.csv</t>
-  </si>
-  <si>
     <t>StorageUnit</t>
   </si>
   <si>
@@ -381,6 +363,39 @@
   </si>
   <si>
     <t>#Store</t>
+  </si>
+  <si>
+    <t>BTES_storage</t>
+  </si>
+  <si>
+    <t>natrium_nuclear</t>
+  </si>
+  <si>
+    <t>natrium_storage</t>
+  </si>
+  <si>
+    <t>natrium_turbine</t>
+  </si>
+  <si>
+    <t>curtailment</t>
+  </si>
+  <si>
+    <t>curtailment_link</t>
+  </si>
+  <si>
+    <t>curtailed_power</t>
+  </si>
+  <si>
+    <t>p_nom</t>
+  </si>
+  <si>
+    <t>20201218_US_mthd3_solar.csv</t>
+  </si>
+  <si>
+    <t>20201218_US_mthd3_wind.csv</t>
+  </si>
+  <si>
+    <t>demand_series_Dan_normalized_to_1_mean_United States.csv</t>
   </si>
 </sst>
 </file>
@@ -1288,10 +1303,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W71"/>
+  <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1546,7 +1561,7 @@
         <v>29</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1554,7 +1569,7 @@
         <v>70</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1570,7 +1585,7 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1578,7 +1593,7 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1586,7 +1601,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" t="s">
@@ -1598,7 +1613,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" s="6"/>
     </row>
@@ -1672,7 +1687,7 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
@@ -1689,7 +1704,7 @@
         <v>75</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" s="1"/>
     </row>
@@ -1733,7 +1748,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="49" spans="1:23" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -1749,41 +1764,44 @@
       <c r="E49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G49" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="G49" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J49" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J49" s="2" t="s">
+      <c r="K49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L49" s="2" t="s">
+      <c r="M49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N49" s="2" t="s">
+      <c r="O49" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O49" s="2" t="s">
+      <c r="P49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P49" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="Q49" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="R49" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R49" s="2" t="s">
+      <c r="S49" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
         <v>35</v>
       </c>
@@ -1794,20 +1812,20 @@
         <v>10</v>
       </c>
       <c r="D50" t="s">
-        <v>87</v>
-      </c>
-      <c r="G50">
+        <v>86</v>
+      </c>
+      <c r="H50">
         <v>1</v>
       </c>
-      <c r="H50" t="s">
-        <v>110</v>
-      </c>
-      <c r="J50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="O50" s="5"/>
+      <c r="I50" t="s">
+        <v>120</v>
+      </c>
+      <c r="K50" s="5"/>
+      <c r="M50" s="5"/>
       <c r="P50" s="5"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q50" s="5"/>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>34</v>
       </c>
@@ -1818,28 +1836,28 @@
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>87</v>
-      </c>
-      <c r="I51" t="s">
-        <v>102</v>
-      </c>
-      <c r="J51" s="18">
+        <v>86</v>
+      </c>
+      <c r="J51" t="s">
+        <v>118</v>
+      </c>
+      <c r="K51" s="18">
         <f>0.014772123*1000*B34</f>
         <v>129403.79748000001</v>
       </c>
-      <c r="K51" t="str">
+      <c r="L51" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L51" s="5"/>
-      <c r="M51" t="str">
+      <c r="M51" s="5"/>
+      <c r="N51" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="O51" s="5"/>
       <c r="P51" s="5"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q51" s="5"/>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>34</v>
       </c>
@@ -1850,30 +1868,30 @@
         <v>22</v>
       </c>
       <c r="D52" t="s">
-        <v>87</v>
-      </c>
-      <c r="I52" t="s">
-        <v>101</v>
-      </c>
-      <c r="J52" s="18">
+        <v>86</v>
+      </c>
+      <c r="J52" t="s">
+        <v>119</v>
+      </c>
+      <c r="K52" s="18">
         <f>0.015913707*1000*B34</f>
         <v>139404.07332</v>
       </c>
-      <c r="K52" t="str">
+      <c r="L52" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L52" s="5"/>
-      <c r="M52" t="str">
+      <c r="M52" s="5"/>
+      <c r="N52" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="O52" s="5"/>
       <c r="P52" s="5"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q52" s="5"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B53" t="s">
         <v>21</v>
@@ -1882,24 +1900,30 @@
         <v>21</v>
       </c>
       <c r="D53" t="s">
-        <v>87</v>
-      </c>
-      <c r="J53" s="15"/>
-      <c r="K53" t="str">
+        <v>86</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53" s="15"/>
+      <c r="L53" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L53" s="5"/>
-      <c r="M53" t="str">
+      <c r="M53" s="5"/>
+      <c r="N53" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="O53" s="5"/>
       <c r="P53" s="5"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q53" s="5"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B54" t="s">
         <v>77</v>
@@ -1908,24 +1932,24 @@
         <v>19</v>
       </c>
       <c r="D54" t="s">
-        <v>87</v>
-      </c>
-      <c r="J54" s="15"/>
-      <c r="K54" t="str">
+        <v>86</v>
+      </c>
+      <c r="K54" s="15"/>
+      <c r="L54" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L54" s="5"/>
-      <c r="M54" t="str">
+      <c r="M54" s="5"/>
+      <c r="N54" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="O54" s="5"/>
       <c r="P54" s="5"/>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q54" s="5"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B55" t="s">
         <v>80</v>
@@ -1934,323 +1958,380 @@
         <v>80</v>
       </c>
       <c r="D55" t="s">
-        <v>87</v>
-      </c>
-      <c r="J55" s="15"/>
-      <c r="K55" t="str">
+        <v>86</v>
+      </c>
+      <c r="K55" s="15"/>
+      <c r="L55" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L55" s="5"/>
-      <c r="M55" t="str">
+      <c r="M55" s="5"/>
+      <c r="N55" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="O55" s="5"/>
       <c r="P55" s="5"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q55" s="5"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B56" t="s">
+        <v>84</v>
+      </c>
+      <c r="C56" t="s">
         <v>85</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>86</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>87</v>
       </c>
-      <c r="E56" t="s">
-        <v>88</v>
-      </c>
-      <c r="F56">
+      <c r="G56">
         <v>-1</v>
       </c>
-      <c r="J56" s="5"/>
-      <c r="K56" t="str">
+      <c r="K56" s="5"/>
+      <c r="L56" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L56" s="5"/>
-      <c r="M56" t="str">
+      <c r="M56" s="5"/>
+      <c r="N56" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="O56" s="5"/>
       <c r="P56" s="5"/>
-      <c r="S56" s="5"/>
-      <c r="W56" s="5"/>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q56" s="5"/>
+      <c r="T56" s="5"/>
+      <c r="X56" s="5"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D57" t="s">
-        <v>88</v>
-      </c>
-      <c r="J57" s="18">
+        <v>87</v>
+      </c>
+      <c r="K57" s="18">
         <f>0.007351353*1000*B34</f>
         <v>64397.852279999999</v>
       </c>
-      <c r="K57" t="str">
+      <c r="L57" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L57" s="20">
+      <c r="M57" s="20">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="M57" t="str">
+      <c r="N57" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="N57" t="b">
+      <c r="O57" t="b">
         <v>1</v>
       </c>
-      <c r="O57" s="5">
+      <c r="P57" s="5">
         <v>0.9</v>
       </c>
-      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
       <c r="R57">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="S57">
         <v>4</v>
       </c>
-      <c r="S57" s="5"/>
-      <c r="W57" s="5"/>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="T57" s="5"/>
+      <c r="X57" s="5"/>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C58" t="s">
         <v>81</v>
       </c>
       <c r="D58" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E58" t="s">
-        <v>83</v>
-      </c>
-      <c r="J58" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="K58" t="str">
+        <v>82</v>
+      </c>
+      <c r="K58" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="L58" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L58" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="M58" t="str">
+      <c r="M58" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="N58" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="O58" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="P58" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="Q58" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A59" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B59" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="C59" t="s">
         <v>81</v>
       </c>
       <c r="D59" t="s">
-        <v>83</v>
-      </c>
-      <c r="J59" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="K59" t="str">
+        <v>82</v>
+      </c>
+      <c r="K59" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="L59" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L59" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="M59" t="str">
+      <c r="M59" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="N59" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="N59" t="b">
+      <c r="O59" t="b">
         <v>1</v>
       </c>
-      <c r="O59" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="P59" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="Q59" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A60" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C60" t="s">
         <v>81</v>
       </c>
       <c r="D60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E60" t="s">
-        <v>114</v>
-      </c>
-      <c r="J60" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="K60" t="str">
+        <v>108</v>
+      </c>
+      <c r="K60" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="L60" t="str">
         <f>B42 &amp; "/time range/" &amp; B41</f>
         <v>$/time range/MW</v>
       </c>
-      <c r="L60" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="M60" t="str">
+      <c r="M60" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="N60" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="O60" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="P60" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="Q60" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D61" t="s">
-        <v>87</v>
-      </c>
-      <c r="J61" s="15"/>
-      <c r="L61" s="5">
+        <v>86</v>
+      </c>
+      <c r="K61" s="15"/>
+      <c r="M61" s="5">
         <v>10000</v>
       </c>
-      <c r="M61" t="str">
+      <c r="N61" t="str">
         <f xml:space="preserve"> B42 &amp; "/" &amp; B41 &amp; B40</f>
         <v>$/MWh</v>
       </c>
-      <c r="O61" s="5"/>
       <c r="P61" s="5"/>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q61" s="5"/>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A62" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B62" t="s">
-        <v>104</v>
+        <v>111</v>
+      </c>
+      <c r="C62" t="s">
+        <v>100</v>
       </c>
       <c r="D62" t="s">
-        <v>114</v>
-      </c>
-      <c r="J62" s="15">
+        <v>108</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62" s="15">
         <f>0.020828805*1000*B34</f>
         <v>182460.33179999999</v>
       </c>
-      <c r="L62" s="5"/>
-      <c r="O62" s="5"/>
+      <c r="M62" s="5"/>
       <c r="P62" s="5"/>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q62" s="5"/>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A63" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>103</v>
+        <v>112</v>
+      </c>
+      <c r="C63" t="s">
+        <v>100</v>
       </c>
       <c r="D63" t="s">
-        <v>114</v>
-      </c>
-      <c r="J63" s="19">
+        <v>108</v>
+      </c>
+      <c r="K63" s="19">
         <f>0.000254017*1000*B34</f>
         <v>2225.1889200000001</v>
       </c>
-      <c r="L63" s="17">
+      <c r="M63" s="17">
         <f>0.00000000371*1000</f>
         <v>3.7099999999999996E-6</v>
       </c>
-      <c r="O63" s="5"/>
       <c r="P63" s="5"/>
-      <c r="Q63" s="16">
+      <c r="Q63" s="5"/>
+      <c r="R63" s="16">
         <v>2.6153100000000001E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A64" s="6" t="s">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>105</v>
+        <v>113</v>
+      </c>
+      <c r="C64" t="s">
+        <v>100</v>
       </c>
       <c r="D64" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E64" t="s">
-        <v>87</v>
-      </c>
-      <c r="J64" s="19">
+        <v>86</v>
+      </c>
+      <c r="K64" s="19">
         <f>0.020905199*1000*B34</f>
         <v>183129.54324</v>
       </c>
-      <c r="L64" s="5"/>
-      <c r="O64" s="16">
+      <c r="M64" s="5"/>
+      <c r="P64" s="16">
         <v>0.37080028399999998</v>
       </c>
-      <c r="P64" s="5"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="Q64" s="5"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" t="s">
+        <v>115</v>
+      </c>
+      <c r="C65" t="s">
+        <v>114</v>
+      </c>
+      <c r="D65" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" t="s">
+        <v>116</v>
+      </c>
+      <c r="K65" s="19"/>
+      <c r="M65" s="5"/>
+      <c r="P65" s="16"/>
+      <c r="Q65" s="5"/>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A66" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" t="s">
+        <v>114</v>
+      </c>
+      <c r="D66" t="s">
+        <v>116</v>
+      </c>
+      <c r="K66" s="19"/>
+      <c r="M66" s="5"/>
+      <c r="P66" s="16"/>
+      <c r="Q66" s="5"/>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A70" s="10" t="s">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A72" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="L70" s="7"/>
-      <c r="M70" s="7"/>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>59</v>
       </c>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7"/>
+      <c r="L73" s="7"/>
+      <c r="M73" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>